<commit_message>
[MCP-181] Addition of new 'mark_for_complexity_is_unchecked' error report.
</commit_message>
<xml_diff>
--- a/sample-data/7510_ureterolithiasis_sc.xlsx
+++ b/sample-data/7510_ureterolithiasis_sc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconroy\Documents\MCP Project\Data Mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD6B06B-B5A3-496F-9007-E21749F23CB0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3DC46E-4C43-6F45-9E8A-7E39DBA61B81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -759,27 +759,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.9296875" customWidth="1"/>
-    <col min="3" max="3" width="29.796875" customWidth="1"/>
-    <col min="4" max="4" width="18.1328125" customWidth="1"/>
-    <col min="5" max="5" width="75.3984375" customWidth="1"/>
-    <col min="6" max="6" width="17.86328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="75.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="19.46484375" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -808,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -831,7 +831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -857,7 +857,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -883,7 +883,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -906,7 +906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -929,7 +929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -952,7 +952,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -975,7 +975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -998,7 +998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="114" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>31</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>32</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -1629,15 +1629,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED79F0EC3E5F7247B5468DE2217405EE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b0145cebf11610b3540f9df2faf3a333">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71f3003f-14ae-4fd3-ad87-6fa34bd771ad" xmlns:ns3="bf4ccbb4-a8ef-483a-aefe-5e3e6c720a8e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0ffa6e98728e15f31cc3911c2059b17" ns2:_="" ns3:_="">
     <xsd:import namespace="71f3003f-14ae-4fd3-ad87-6fa34bd771ad"/>
@@ -1854,6 +1845,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1861,14 +1861,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3A57279-E5D5-47C4-975E-BFFA068B42C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2DF119B-39D7-42AD-AC0A-3374EF364CB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1883,6 +1875,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3A57279-E5D5-47C4-975E-BFFA068B42C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>